<commit_message>
generating report. temporary version
</commit_message>
<xml_diff>
--- a/productiveedge.xlsx
+++ b/productiveedge.xlsx
@@ -44,7 +44,7 @@
     <t>parentURLs</t>
   </si>
   <si>
-    <t>https://www.productiveedge.com/</t>
+    <t>https://www.productiveedge.com</t>
   </si>
   <si>
     <t>PROCESSED</t>
@@ -59,13 +59,13 @@
     <t>[https://goo.gl/maps/c3hgman3qps, https://blog.productiveedge.com/, http://www.facebook.com/productiveedge, https://www.linkedin.com/company/productive-edge-llc-, https://twitter.com/productiveedge]</t>
   </si>
   <si>
-    <t>[https://www.productiveedge.com/company/office-locations, https://www.productiveedge.com/technology/artificial-intelligence, https://www.productiveedge.com/solutions/intranets-portals, https://www.productiveedge.com/solutions/marketing-transformation, https://www.productiveedge.com/technology/intelligent-automation, https://www.productiveedge.com/case-study/iot-preventative-cs, https://www.productiveedge.com/technology/blockchain, https://www.productiveedge.com/solutions/intelligent-automation, https://www.productiveedge.com/solutions/immersive-experiences, https://www.productiveedge.com/company/portfolio, https://www.productiveedge.com/company/culture, https://www.productiveedge.com/company/strategic-partnerships, https://www.productiveedge.com/, https://www.productiveedge.com/customer-experience, https://www.productiveedge.com/blog/roadblocks-smart-services/, https://www.productiveedge.com/blog, https://www.productiveedge.com/contact-us, https://www.productiveedge.com/digital-strategy, https://www.productiveedge.com/case-study/law-cs, https://www.productiveedge.com/blog/digital-marketing-challenges/, https://www.productiveedge.com/company/team, https://www.productiveedge.com/privacy, https://www.productiveedge.com/blog/organization-ready-dxp/, https://www.productiveedge.com/insights/content-library, https://www.productiveedge.com/technology/cloud, https://www.productiveedge.com/technology/sitecore, https://www.productiveedge.com/solutions/smart-services, https://www.productiveedge.com/technology/xamarin, https://www.productiveedge.com/solutions/operationalizing-ai, https://www.productiveedge.com/terms-of-use, https://www.productiveedge.com/technology/iot, https://www.productiveedge.com/technology/magnolia, https://www.productiveedge.com/case-study/cruise-line-cs, https://www.productiveedge.com/technology/ar-vr, https://www.productiveedge.com/careers, https://www.productiveedge.com/solutions/modern-mobility, https://www.productiveedge.com/case-study/hockey-experience-cs, https://www.productiveedge.com/company/recognition-awards]</t>
+    <t>[https://www.productiveedge.com/company/office-locations, https://www.productiveedge.com/technology/artificial-intelligence, https://www.productiveedge.com/solutions/intranets-portals, https://www.productiveedge.com/solutions/marketing-transformation, https://www.productiveedge.com/technology/intelligent-automation, https://www.productiveedge.com/case-study/iot-preventative-cs, https://www.productiveedge.com/technology/blockchain, https://www.productiveedge.com/solutions/intelligent-automation, https://www.productiveedge.com/solutions/immersive-experiences, https://www.productiveedge.com/company/portfolio, https://www.productiveedge.com/company/culture, https://www.productiveedge.com/company/strategic-partnerships, https://www.productiveedge.com/, https://www.productiveedge.com/customer-experience, https://www.productiveedge.com/blog/roadblocks-smart-services/, https://www.productiveedge.com/blog, https://www.productiveedge.com/contact-us, https://www.productiveedge.com/digital-strategy, https://www.productiveedge.com/case-study/law-cs, https://www.productiveedge.com/blog/digital-marketing-challenges/, https://www.productiveedge.com/company/team, https://www.productiveedge.com/privacy, https://www.productiveedge.com/blog/organization-ready-dxp/, https://www.productiveedge.com/insights/content-library, https://www.productiveedge.com/technology/cloud, https://www.productiveedge.com/technology/sitecore, https://www.productiveedge.com/solutions/smart-services, https://www.productiveedge.com/technology/xamarin, https://www.productiveedge.com/solutions/operationalizing-ai, https://www.productiveedge.com/terms-of-use, https://www.productiveedge.com/technology/iot, https://www.productiveedge.com/technology/magnolia, https://www.productiveedge.com/case-study/cruise-line-cs, https://www.productiveedge.com/technology/ar-vr, https://www.productiveedge.com/careers, https://www.productiveedge.com/solutions/modern-mobility, https://www.productiveedge.com, https://www.productiveedge.com/case-study/hockey-experience-cs, https://www.productiveedge.com/company/recognition-awards]</t>
   </si>
   <si>
     <t>[]</t>
   </si>
   <si>
-    <t>[https://www.productiveedge.com/company/office-locations, https://www.productiveedge.com/solutions/intranets-portals, https://www.productiveedge.com/solutions/marketing-transformation, https://www.productiveedge.com/technology/artificial-intelligence, https://www.productiveedge.com/technology/intelligent-automation, https://www.productiveedge.com/case-study/iot-preventative-cs, https://www.productiveedge.com/case-study/beauty-cs, https://www.productiveedge.com/case-study/observatory-cs, https://www.productiveedge.com/technology/blockchain, https://www.productiveedge.com/solutions/immersive-experiences, https://www.productiveedge.com/solutions/intelligent-automation, https://www.productiveedge.com/company/culture, https://www.productiveedge.com/company/strategic-partnerships, https://www.productiveedge.com/, https://www.productiveedge.com/case-study/caregiver-cs, https://www.productiveedge.com/case-study/health-insurance-cs, https://www.productiveedge.com/customer-experience, https://www.productiveedge.com/contact-us, https://www.productiveedge.com/case-study/law-cs, https://www.productiveedge.com/digital-strategy, https://www.productiveedge.com/company/team, https://www.productiveedge.com/privacy, https://www.productiveedge.com/case-study/rx-automation-cs, https://www.productiveedge.com/technology/cloud, https://www.productiveedge.com/solutions/smart-services, https://www.productiveedge.com/technology/sitecore, https://www.productiveedge.com/technology/xamarin, https://www.productiveedge.com/solutions/operationalizing-ai, https://www.productiveedge.com/terms-of-use, https://www.productiveedge.com/technology/iot, https://www.productiveedge.com/technology/magnolia, https://www.productiveedge.com/case-study/cruise-line-cs, https://www.productiveedge.com/technology/ar-vr, https://www.productiveedge.com/careers, https://www.productiveedge.com/solutions/modern-mobility, https://www.productiveedge.com/case-study/insurance-health-cs, https://www.productiveedge.com/case-study/hockey-experience-cs, https://www.productiveedge.com/company/recognition-awards]</t>
+    <t>[https://www.productiveedge.com/company/office-locations, https://www.productiveedge.com/solutions/intranets-portals, https://www.productiveedge.com/solutions/marketing-transformation, https://www.productiveedge.com/technology/artificial-intelligence, https://www.productiveedge.com/technology/intelligent-automation, https://www.productiveedge.com/case-study/iot-preventative-cs, https://www.productiveedge.com/case-study/beauty-cs, https://www.productiveedge.com/case-study/observatory-cs, https://www.productiveedge.com/technology/blockchain, https://www.productiveedge.com/solutions/immersive-experiences, https://www.productiveedge.com/solutions/intelligent-automation, https://www.productiveedge.com/company/culture, https://www.productiveedge.com/company/strategic-partnerships, https://www.productiveedge.com/case-study/caregiver-cs, https://www.productiveedge.com/case-study/health-insurance-cs, https://www.productiveedge.com/customer-experience, https://www.productiveedge.com/contact-us, https://www.productiveedge.com/case-study/law-cs, https://www.productiveedge.com/digital-strategy, https://www.productiveedge.com/company/team, https://www.productiveedge.com/privacy, https://www.productiveedge.com/case-study/rx-automation-cs, https://www.productiveedge.com/technology/cloud, https://www.productiveedge.com/solutions/smart-services, https://www.productiveedge.com/technology/sitecore, https://www.productiveedge.com/technology/xamarin, https://www.productiveedge.com/solutions/operationalizing-ai, https://www.productiveedge.com/terms-of-use, https://www.productiveedge.com/technology/iot, https://www.productiveedge.com/technology/magnolia, https://www.productiveedge.com/case-study/cruise-line-cs, https://www.productiveedge.com/technology/ar-vr, https://www.productiveedge.com/careers, https://www.productiveedge.com/solutions/modern-mobility, https://www.productiveedge.com, https://www.productiveedge.com/case-study/insurance-health-cs, https://www.productiveedge.com/case-study/hockey-experience-cs, https://www.productiveedge.com/company/recognition-awards]</t>
   </si>
   <si>
     <t>https://www.productiveedge.com/blog</t>
@@ -254,7 +254,7 @@
     <t>[https://www.productiveedge.com/company/office-locations, https://www.productiveedge.com/technology/artificial-intelligence, https://www.productiveedge.com/solutions/intranets-portals, https://www.productiveedge.com/solutions/marketing-transformation, https://www.productiveedge.com/technology/intelligent-automation, https://www.productiveedge.com/technology/blockchain, https://www.productiveedge.com/solutions/intelligent-automation, https://www.productiveedge.com/solutions/immersive-experiences, https://www.productiveedge.com/company/portfolio, https://www.productiveedge.com/company/culture, https://www.productiveedge.com/company/strategic-partnerships, https://www.productiveedge.com/, https://www.productiveedge.com/customer-experience, https://www.productiveedge.com/contact-us, https://www.productiveedge.com/digital-strategy, https://www.productiveedge.com/company/team, https://www.productiveedge.com/privacy, https://www.productiveedge.com/insights/content-library, https://www.productiveedge.com/technology/cloud, https://www.productiveedge.com/technology/sitecore, https://www.productiveedge.com/solutions/smart-services, https://www.productiveedge.com/technology/xamarin, https://www.productiveedge.com/solutions/operationalizing-ai, https://www.productiveedge.com/terms-of-use, https://www.productiveedge.com/technology/iot, https://www.productiveedge.com/technology/magnolia, https://www.productiveedge.com/case-study/cruise-line-cs, https://www.productiveedge.com/technology/ar-vr, https://www.productiveedge.com/careers, https://www.productiveedge.com/solutions/modern-mobility, https://www.productiveedge.com/company/recognition-awards]</t>
   </si>
   <si>
-    <t>[https://www.productiveedge.com/solutions/marketing-transformation, https://www.productiveedge.com/, https://www.productiveedge.com/technology/magnolia, https://www.productiveedge.com/case-study/cruise-line-cs, https://www.productiveedge.com/company/recognition-awards]</t>
+    <t>[https://www.productiveedge.com/solutions/marketing-transformation, https://www.productiveedge.com/technology/magnolia, https://www.productiveedge.com/case-study/cruise-line-cs, https://www.productiveedge.com, https://www.productiveedge.com/company/recognition-awards]</t>
   </si>
   <si>
     <t>https://www.productiveedge.com/case-study/health-insurance-cs</t>
@@ -272,7 +272,7 @@
     <t>[https://www.productiveedge.com/company/office-locations, https://www.productiveedge.com/technology/artificial-intelligence, https://www.productiveedge.com/solutions/intranets-portals, https://www.productiveedge.com/solutions/marketing-transformation, https://www.productiveedge.com/technology/intelligent-automation, https://www.productiveedge.com/technology/blockchain, https://www.productiveedge.com/solutions/intelligent-automation, https://www.productiveedge.com/solutions/immersive-experiences, https://www.productiveedge.com/company/portfolio, https://www.productiveedge.com/company/culture, https://www.productiveedge.com/company/strategic-partnerships, https://www.productiveedge.com/, https://www.productiveedge.com/customer-experience, https://www.productiveedge.com/contact-us, https://www.productiveedge.com/digital-strategy, https://www.productiveedge.com/company/team, https://www.productiveedge.com/privacy, https://www.productiveedge.com/insights/content-library, https://www.productiveedge.com/technology/cloud, https://www.productiveedge.com/technology/sitecore, https://www.productiveedge.com/solutions/smart-services, https://www.productiveedge.com/technology/xamarin, https://www.productiveedge.com/solutions/operationalizing-ai, https://www.productiveedge.com/terms-of-use, https://www.productiveedge.com/technology/iot, https://www.productiveedge.com/technology/magnolia, https://www.productiveedge.com/technology/ar-vr, https://www.productiveedge.com/careers, https://www.productiveedge.com/solutions/modern-mobility, https://www.productiveedge.com/case-study/hockey-experience-cs, https://www.productiveedge.com/company/recognition-awards]</t>
   </si>
   <si>
-    <t>[https://www.productiveedge.com/, https://www.productiveedge.com/technology/ar-vr, https://www.productiveedge.com/solutions/immersive-experiences, https://www.productiveedge.com/case-study/hockey-experience-cs]</t>
+    <t>[https://www.productiveedge.com/technology/ar-vr, https://www.productiveedge.com/solutions/immersive-experiences, https://www.productiveedge.com, https://www.productiveedge.com/case-study/hockey-experience-cs]</t>
   </si>
   <si>
     <t>https://www.productiveedge.com/case-study/insurance-health-cs</t>
@@ -290,7 +290,7 @@
     <t>[https://www.productiveedge.com/company/office-locations, https://www.productiveedge.com/technology/artificial-intelligence, https://www.productiveedge.com/solutions/intranets-portals, https://www.productiveedge.com/solutions/marketing-transformation, https://www.productiveedge.com/technology/intelligent-automation, https://www.productiveedge.com/case-study/iot-preventative-cs, https://www.productiveedge.com/technology/blockchain, https://www.productiveedge.com/solutions/intelligent-automation, https://www.productiveedge.com/solutions/immersive-experiences, https://www.productiveedge.com/company/portfolio, https://www.productiveedge.com/company/culture, https://www.productiveedge.com/company/strategic-partnerships, https://www.productiveedge.com/, https://www.productiveedge.com/customer-experience, https://www.productiveedge.com/contact-us, https://www.productiveedge.com/digital-strategy, https://www.productiveedge.com/company/team, https://www.productiveedge.com/privacy, https://www.productiveedge.com/insights/content-library, https://www.productiveedge.com/technology/cloud, https://www.productiveedge.com/technology/sitecore, https://www.productiveedge.com/solutions/smart-services, https://www.productiveedge.com/technology/xamarin, https://www.productiveedge.com/solutions/operationalizing-ai, https://www.productiveedge.com/terms-of-use, https://www.productiveedge.com/technology/iot, https://www.productiveedge.com/technology/magnolia, https://www.productiveedge.com/technology/ar-vr, https://www.productiveedge.com/careers, https://www.productiveedge.com/solutions/modern-mobility, https://www.productiveedge.com/company/recognition-awards]</t>
   </si>
   <si>
-    <t>[https://www.productiveedge.com/, https://www.productiveedge.com/case-study/iot-preventative-cs]</t>
+    <t>[https://www.productiveedge.com/case-study/iot-preventative-cs, https://www.productiveedge.com]</t>
   </si>
   <si>
     <t>https://www.productiveedge.com/case-study/law-cs</t>
@@ -299,7 +299,7 @@
     <t>[https://www.productiveedge.com/company/office-locations, https://www.productiveedge.com/technology/artificial-intelligence, https://www.productiveedge.com/solutions/intranets-portals, https://www.productiveedge.com/solutions/marketing-transformation, https://www.productiveedge.com/technology/intelligent-automation, https://www.productiveedge.com/technology/blockchain, https://www.productiveedge.com/solutions/intelligent-automation, https://www.productiveedge.com/solutions/immersive-experiences, https://www.productiveedge.com/company/portfolio, https://www.productiveedge.com/company/culture, https://www.productiveedge.com/company/strategic-partnerships, https://www.productiveedge.com/, https://www.productiveedge.com/customer-experience, https://www.productiveedge.com/contact-us, https://www.productiveedge.com/case-study/law-cs, https://www.productiveedge.com/digital-strategy, https://www.productiveedge.com/company/team, https://www.productiveedge.com/privacy, https://www.productiveedge.com/insights/content-library, https://www.productiveedge.com/technology/cloud, https://www.productiveedge.com/technology/sitecore, https://www.productiveedge.com/solutions/smart-services, https://www.productiveedge.com/technology/xamarin, https://www.productiveedge.com/solutions/operationalizing-ai, https://www.productiveedge.com/terms-of-use, https://www.productiveedge.com/technology/iot, https://www.productiveedge.com/technology/magnolia, https://www.productiveedge.com/technology/ar-vr, https://www.productiveedge.com/careers, https://www.productiveedge.com/solutions/modern-mobility, https://www.productiveedge.com/company/recognition-awards]</t>
   </si>
   <si>
-    <t>[https://www.productiveedge.com/solutions/intranets-portals, https://www.productiveedge.com/, https://www.productiveedge.com/technology/sitecore, https://www.productiveedge.com/case-study/law-cs]</t>
+    <t>[https://www.productiveedge.com/solutions/intranets-portals, https://www.productiveedge.com/technology/sitecore, https://www.productiveedge.com, https://www.productiveedge.com/case-study/law-cs]</t>
   </si>
   <si>
     <t>https://www.productiveedge.com/case-study/observatory-cs</t>
@@ -516,10 +516,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>

</xml_diff>